<commit_message>
Added patterns to documention. Added Route State Identifier project.
</commit_message>
<xml_diff>
--- a/RMSXRouteFillTest/RMSXRouteFillTest_SequenceDiagram.xlsx
+++ b/RMSXRouteFillTest/RMSXRouteFillTest_SequenceDiagram.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="SequenceDiagram" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="EMSX Patterns" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="139">
   <si>
     <t xml:space="preserve">RouteFillTest</t>
   </si>
@@ -299,6 +300,150 @@
   </si>
   <si>
     <t xml:space="preserve">Call Evaluate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Previous Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meaning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMSX_STATUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New route created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working amount set on route (can be ignored)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMSX_WORKING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WORKING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACK received from broker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARTFILL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First fill of multiple fills (&lt; 100%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;n and &gt;0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Middle fill of multiple fills (&lt; 100%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FILLED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final fill of multiple fills (100%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full single fill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Historic 100% fill on INIT_PAINT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working route on INIT_PAINT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part filled route on INIT_PAINT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CXLREQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancel requested on route in INIT_PAINT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancel route request sent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broker rejected cancel request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CXLPEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broker sent ACK for cancel request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CANCEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broker cancelled route from request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broker cancelled route from pending status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancel requested on part filled route</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broker rejected cancel request on part filled route</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CXLRPRQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modify (cancel/replace) request sent to broker on working route</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REPPEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broker sent ACK for modify request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broker rejected modify request on working route</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMSX_BROKER_STATUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CXLRPRJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broker accepted and applied the modify request on working route</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MODIFIED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modify (cancel/replace) request sent to broker on part filled route</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broker rejected modify request on part filled route</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broker accepted and applied the modify request on part filled route</t>
   </si>
 </sst>
 </file>
@@ -308,7 +453,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -344,16 +489,45 @@
       <name val="Calibri"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0084D1"/>
+        <bgColor rgb="FF008080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE7F5"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="14">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -403,6 +577,55 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -429,7 +652,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="44">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -478,6 +701,134 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -508,10 +859,10 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCFE7F5"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF0084D1"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -561,9 +912,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>550080</xdr:colOff>
+      <xdr:colOff>549720</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>116280</xdr:rowOff>
+      <xdr:rowOff>115920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -573,7 +924,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="698400" y="1886040"/>
-          <a:ext cx="10986120" cy="20880"/>
+          <a:ext cx="10982520" cy="20520"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -625,9 +976,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>825480</xdr:colOff>
+      <xdr:colOff>825120</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>107280</xdr:rowOff>
+      <xdr:rowOff>106920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -636,8 +987,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11716920" y="2838600"/>
-          <a:ext cx="10974600" cy="11880"/>
+          <a:off x="11713680" y="2838600"/>
+          <a:ext cx="10971000" cy="11520"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -683,13 +1034,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>528840</xdr:colOff>
+      <xdr:colOff>528120</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>105840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>771840</xdr:colOff>
+      <xdr:colOff>770760</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>106200</xdr:rowOff>
     </xdr:to>
@@ -700,8 +1051,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="11663280" y="3039480"/>
-          <a:ext cx="10974600" cy="360"/>
+          <a:off x="11659320" y="3039480"/>
+          <a:ext cx="10971000" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -753,9 +1104,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>528480</xdr:colOff>
+      <xdr:colOff>528120</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>99360</xdr:rowOff>
+      <xdr:rowOff>99000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -765,7 +1116,7 @@
       <xdr:spPr>
         <a:xfrm flipH="1">
           <a:off x="659880" y="3524400"/>
-          <a:ext cx="11003040" cy="3960"/>
+          <a:ext cx="10999440" cy="3600"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -811,15 +1162,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>-23217480</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:colOff>702720</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>78120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>713160</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>95400</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>740160</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -827,9 +1178,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="-23217480" y="3686040"/>
-          <a:ext cx="23930640" cy="14400"/>
+        <a:xfrm>
+          <a:off x="702720" y="4878720"/>
+          <a:ext cx="13889880" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -875,15 +1226,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>-23226120</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:colOff>635040</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>74160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>676800</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>95400</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>644760</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -891,9 +1242,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="-23226120" y="3895200"/>
-          <a:ext cx="23902920" cy="10080"/>
+        <a:xfrm flipH="1">
+          <a:off x="635040" y="5027040"/>
+          <a:ext cx="13862160" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -939,15 +1290,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>702720</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>78120</xdr:rowOff>
+      <xdr:colOff>622800</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>740520</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>78480</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>717480</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>74880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -955,9 +1306,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="702720" y="4878720"/>
-          <a:ext cx="13893480" cy="360"/>
+        <a:xfrm flipH="1">
+          <a:off x="622800" y="5636880"/>
+          <a:ext cx="30365640" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1003,15 +1354,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>635040</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>74160</xdr:rowOff>
+      <xdr:colOff>690120</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>65520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>645120</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>74520</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>718920</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>73440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1019,9 +1370,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="635040" y="5027040"/>
-          <a:ext cx="13865760" cy="360"/>
+        <a:xfrm>
+          <a:off x="690120" y="6237720"/>
+          <a:ext cx="31901040" cy="7920"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1067,15 +1418,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>-29648880</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>50760</xdr:rowOff>
+      <xdr:colOff>633600</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>88920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>696240</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>66240</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>658440</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>94680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1083,9 +1434,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="-29648880" y="5140440"/>
-          <a:ext cx="30345120" cy="15480"/>
+        <a:xfrm flipH="1">
+          <a:off x="633600" y="6718320"/>
+          <a:ext cx="31897080" cy="5760"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1130,16 +1481,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>623520</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>74520</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>624960</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>718560</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>687600</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1147,9 +1498,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="623520" y="5636880"/>
-          <a:ext cx="30375000" cy="360"/>
+        <a:xfrm flipV="1">
+          <a:off x="29294280" y="6396480"/>
+          <a:ext cx="3265560" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1194,16 +1545,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>690120</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>65520</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>635040</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>72720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>719280</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>73800</xdr:rowOff>
+      <xdr:colOff>655560</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>73080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1211,9 +1562,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="690120" y="6237720"/>
-          <a:ext cx="31911120" cy="8280"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="29304360" y="6549480"/>
+          <a:ext cx="3223440" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1259,15 +1610,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>634320</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>88920</xdr:rowOff>
+      <xdr:colOff>694440</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>70200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>659520</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>95040</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>750960</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>70560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1275,9 +1626,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="634320" y="6718320"/>
-          <a:ext cx="31907160" cy="6120"/>
+        <a:xfrm>
+          <a:off x="694440" y="7461360"/>
+          <a:ext cx="36733320" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1322,16 +1673,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>624960</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>73080</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>650160</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>87120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>687960</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>73440</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>712800</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>87480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1340,8 +1691,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="29302560" y="6397200"/>
-          <a:ext cx="3267360" cy="360"/>
+          <a:off x="34124040" y="7630560"/>
+          <a:ext cx="3265560" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1386,16 +1737,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>635040</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>73440</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>660240</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>76680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>655920</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>73800</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>680760</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1404,8 +1755,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="29312640" y="6550200"/>
-          <a:ext cx="3225240" cy="360"/>
+          <a:off x="34134120" y="7772760"/>
+          <a:ext cx="3223440" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1451,15 +1802,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>694440</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>70200</xdr:rowOff>
+      <xdr:colOff>634320</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>751320</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>70560</xdr:rowOff>
+      <xdr:colOff>712080</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>78840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1467,9 +1818,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="694440" y="7461360"/>
-          <a:ext cx="36745200" cy="360"/>
+        <a:xfrm flipH="1">
+          <a:off x="634320" y="7926840"/>
+          <a:ext cx="36754560" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1514,16 +1865,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>650160</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>87840</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>698040</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>84600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>713160</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>88200</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>718560</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>84960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1531,9 +1882,73 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2158920" y="9609480"/>
+          <a:ext cx="15615000" cy="360"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="21600" h="21600">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="21600" y="21600"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="34920">
+          <a:solidFill>
+            <a:srgbClr val="ffffff"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd len="med" type="oval" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>577080</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>66240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>755640</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>66600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="34134120" y="7631280"/>
-          <a:ext cx="3267360" cy="360"/>
+          <a:off x="577080" y="9743040"/>
+          <a:ext cx="1639440" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1578,26 +1993,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>660240</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>77400</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>642240</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>70200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>681120</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>77760</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>707040</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>70560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="CustomShape 1"/>
+        <xdr:cNvPr id="17" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="34144200" y="7773480"/>
-          <a:ext cx="3225240" cy="360"/>
+        <a:xfrm flipV="1">
+          <a:off x="26108640" y="10356840"/>
+          <a:ext cx="8072280" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1642,26 +2057,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>634320</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>78480</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>645480</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>74160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>712440</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>78840</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>707760</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>83880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="CustomShape 1"/>
+        <xdr:cNvPr id="18" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="634320" y="7926840"/>
-          <a:ext cx="36766440" cy="360"/>
+          <a:off x="34119360" y="10513440"/>
+          <a:ext cx="8069760" cy="9720"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1706,80 +2121,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>698760</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>84600</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>708120</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>78840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>719640</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>84960</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="2159640" y="9609480"/>
-          <a:ext cx="15619680" cy="360"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="21600" h="21600">
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="21600" y="21600"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="34920">
-          <a:solidFill>
-            <a:schemeClr val="accent2"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd len="med" type="oval" w="med"/>
-          <a:tailEnd len="med" type="triangle" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>577080</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>66960</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>756000</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>67320</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>712080</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>84600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1787,9 +2138,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="577080" y="9743760"/>
-          <a:ext cx="1639800" cy="360"/>
+        <a:xfrm flipH="1">
+          <a:off x="3770640" y="10670400"/>
+          <a:ext cx="30415320" cy="5760"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1834,16 +2185,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>-26578440</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>60840</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>650520</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>70560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>770400</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>61200</xdr:rowOff>
+      <xdr:colOff>748800</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>70920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1852,8 +2203,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="-26578440" y="10194840"/>
-          <a:ext cx="30412080" cy="360"/>
+          <a:off x="2111400" y="11118960"/>
+          <a:ext cx="1699920" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1898,16 +2249,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>642240</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>70920</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>655920</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>74160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>707400</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>71280</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>729360</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1915,9 +2266,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="26115840" y="10357560"/>
-          <a:ext cx="8075520" cy="360"/>
+        <a:xfrm flipH="1">
+          <a:off x="5381280" y="11732760"/>
+          <a:ext cx="14004720" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1962,16 +2313,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>645480</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>74160</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>697320</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>708120</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>84240</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>722520</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>78840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1980,8 +2331,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="34129440" y="10513440"/>
-          <a:ext cx="8073360" cy="10080"/>
+          <a:off x="3759840" y="11889360"/>
+          <a:ext cx="1688040" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2026,16 +2377,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>708840</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>78840</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>651960</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>713160</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>84960</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>689760</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>74880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2043,9 +2394,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="3772080" y="10670400"/>
-          <a:ext cx="30425040" cy="6120"/>
+        <a:xfrm flipV="1">
+          <a:off x="42133320" y="12189960"/>
+          <a:ext cx="1639080" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2090,16 +2441,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>650520</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>71280</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>623880</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>69840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>749160</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>71640</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>661680</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>70200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2107,9 +2458,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="2111400" y="11119680"/>
-          <a:ext cx="1701000" cy="360"/>
+        <a:xfrm flipH="1">
+          <a:off x="43706520" y="12337920"/>
+          <a:ext cx="1639440" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2154,16 +2505,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>-8559000</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>75600</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>686520</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>711720</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>75960</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>74880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2171,9 +2522,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="-8559000" y="11581200"/>
-          <a:ext cx="13996800" cy="360"/>
+        <a:xfrm flipH="1">
+          <a:off x="3749040" y="12494880"/>
+          <a:ext cx="40019400" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2218,16 +2569,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>655920</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>74160</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>95400</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>53280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>729720</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>74520</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>285120</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>63000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2235,405 +2586,19 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="5382000" y="11732760"/>
-          <a:ext cx="14009400" cy="360"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="21600" h="21600">
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="21600" y="21600"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="34920">
-          <a:solidFill>
-            <a:srgbClr val="4a7ebb"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd len="med" type="oval" w="med"/>
-          <a:tailEnd len="med" type="triangle" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>698040</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>78480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>723600</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>78840</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="27" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="3761280" y="11889360"/>
-          <a:ext cx="1688400" cy="360"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="21600" h="21600">
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="21600" y="21600"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="34920">
-          <a:solidFill>
-            <a:srgbClr val="4a7ebb"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd len="med" type="oval" w="med"/>
-          <a:tailEnd len="med" type="triangle" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>-36216360</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>69120</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>757800</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>69480</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="28" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="-36216360" y="12031920"/>
-          <a:ext cx="40037400" cy="360"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="21600" h="21600">
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="21600" y="21600"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="34920">
-          <a:solidFill>
-            <a:srgbClr val="4a7ebb"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd len="med" type="oval" w="med"/>
-          <a:tailEnd len="med" type="triangle" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>651960</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>75240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>690120</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>75600</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="29" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="42146640" y="12190680"/>
-          <a:ext cx="1640160" cy="360"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="21600" h="21600">
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="21600" y="21600"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="34920">
-          <a:solidFill>
-            <a:srgbClr val="4a7ebb"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd len="med" type="oval" w="med"/>
-          <a:tailEnd len="med" type="triangle" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>623880</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>69840</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>662040</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>70200</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="30" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="43720560" y="12337920"/>
-          <a:ext cx="1640160" cy="360"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="21600" h="21600">
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="21600" y="21600"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="34920">
-          <a:solidFill>
-            <a:srgbClr val="4a7ebb"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd len="med" type="oval" w="med"/>
-          <a:tailEnd len="med" type="triangle" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>687240</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>74520</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>686880</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="31" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="3750480" y="12494880"/>
-          <a:ext cx="40033080" cy="360"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="21600" h="21600">
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="21600" y="21600"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="34920">
-          <a:solidFill>
-            <a:srgbClr val="4a7ebb"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd len="med" type="oval" w="med"/>
-          <a:tailEnd len="med" type="triangle" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>95400</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>53280</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>285480</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>63360</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="32" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
         <a:xfrm>
-          <a:off x="3158640" y="11102040"/>
-          <a:ext cx="190080" cy="1381680"/>
+          <a:off x="3157920" y="11102040"/>
+          <a:ext cx="189720" cy="1381320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
+            <a:srgbClr val="ffffff"/>
           </a:solidFill>
           <a:round/>
         </a:ln>
@@ -2671,26 +2636,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>-31471560</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>75600</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>767160</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>74880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>774720</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>75960</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>764280</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>75240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="33" name="CustomShape 1"/>
+        <xdr:cNvPr id="27" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="-31471560" y="13124160"/>
-          <a:ext cx="35309520" cy="360"/>
+          <a:off x="31038120" y="13428360"/>
+          <a:ext cx="8004240" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2735,26 +2700,90 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>767160</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>75600</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>595440</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>68400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>764640</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>75960</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>694440</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>68760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="34" name="CustomShape 1"/>
+        <xdr:cNvPr id="28" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="31047120" y="13429080"/>
-          <a:ext cx="8007840" cy="360"/>
+          <a:off x="43678080" y="14336280"/>
+          <a:ext cx="3301920" cy="360"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="21600" h="21600">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="21600" y="21600"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="34920">
+          <a:solidFill>
+            <a:srgbClr val="ffffff"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd len="med" type="oval" w="med"/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>733680</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>68400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>747360</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>68760</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="29403000" y="14945760"/>
+          <a:ext cx="9622440" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2799,90 +2828,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>595440</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>69120</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>656280</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>69840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>694800</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>69480</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>693360</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>70200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="35" name="CustomShape 1"/>
+        <xdr:cNvPr id="30" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="43692120" y="14337000"/>
-          <a:ext cx="3303360" cy="360"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="21600" h="21600">
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="21600" y="21600"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="34920">
-          <a:solidFill>
-            <a:schemeClr val="accent2"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd len="med" type="oval" w="med"/>
-          <a:tailEnd len="med" type="triangle" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>733680</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>69120</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>747720</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>69480</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="36" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="29411280" y="14946480"/>
-          <a:ext cx="9626760" cy="360"/>
+        <a:xfrm flipH="1">
+          <a:off x="46941840" y="13728600"/>
+          <a:ext cx="1638720" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2927,26 +2892,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>656280</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>69840</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>697680</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>74160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>693720</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>70200</xdr:rowOff>
+      <xdr:colOff>696600</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="37" name="CustomShape 1"/>
+        <xdr:cNvPr id="31" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="46956960" y="13728600"/>
-          <a:ext cx="1639800" cy="360"/>
+          <a:off x="38975760" y="15104520"/>
+          <a:ext cx="9608040" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2992,25 +2957,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>698400</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>74160</xdr:rowOff>
+      <xdr:colOff>698040</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>78840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>697680</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>74520</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>722880</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>79200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="38" name="CustomShape 1"/>
+        <xdr:cNvPr id="32" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="38988720" y="15104520"/>
-          <a:ext cx="9612000" cy="360"/>
+          <a:off x="38976120" y="13889880"/>
+          <a:ext cx="8032320" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3055,26 +3020,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>698040</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>78840</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>750960</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>70200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>723240</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>79200</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>746280</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>70560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="39" name="CustomShape 1"/>
+        <xdr:cNvPr id="33" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="38988360" y="13889880"/>
-          <a:ext cx="8035560" cy="360"/>
+          <a:off x="3813480" y="15710040"/>
+          <a:ext cx="35210880" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3119,26 +3084,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>750960</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>70200</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>641160</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>746640</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>70560</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>678240</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>77400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="40" name="CustomShape 1"/>
+        <xdr:cNvPr id="34" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="3814200" y="15710040"/>
-          <a:ext cx="35222760" cy="360"/>
+        <a:xfrm flipV="1">
+          <a:off x="45325440" y="16183800"/>
+          <a:ext cx="4841280" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3183,26 +3148,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>641160</xdr:colOff>
-      <xdr:row>88</xdr:row>
-      <xdr:rowOff>77760</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>757080</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>86040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>678600</xdr:colOff>
-      <xdr:row>88</xdr:row>
-      <xdr:rowOff>78120</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>773280</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>86400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="41" name="CustomShape 1"/>
+        <xdr:cNvPr id="35" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="45339840" y="16184520"/>
-          <a:ext cx="4843800" cy="360"/>
+          <a:off x="51847200" y="16802640"/>
+          <a:ext cx="3219120" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3247,26 +3212,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>757080</xdr:colOff>
-      <xdr:row>90</xdr:row>
-      <xdr:rowOff>86760</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>688680</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>86040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>773640</xdr:colOff>
-      <xdr:row>90</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>725760</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>86400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="42" name="CustomShape 1"/>
+        <xdr:cNvPr id="36" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="51864120" y="16803360"/>
-          <a:ext cx="3220920" cy="360"/>
+          <a:off x="56583000" y="16954920"/>
+          <a:ext cx="1638720" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3311,26 +3276,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>688680</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>86760</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>733320</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>79920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>726120</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>695160</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>80280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="43" name="CustomShape 1"/>
+        <xdr:cNvPr id="37" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="56602080" y="16955640"/>
-          <a:ext cx="1639800" cy="360"/>
+        <a:xfrm flipH="1">
+          <a:off x="29402640" y="17558640"/>
+          <a:ext cx="30389760" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3375,26 +3340,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>733320</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>79920</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>679680</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>75960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>695520</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>80280</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>700200</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="44" name="CustomShape 1"/>
+        <xdr:cNvPr id="38" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="29410920" y="17558640"/>
-          <a:ext cx="30402360" cy="360"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="27747720" y="5333760"/>
+          <a:ext cx="3223440" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3440,25 +3405,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>679680</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:colOff>721800</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>79920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>700560</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:colOff>784440</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>80280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="45" name="CustomShape 1"/>
+        <xdr:cNvPr id="39" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="27755280" y="5334480"/>
-          <a:ext cx="3225240" cy="360"/>
+        <a:xfrm flipV="1">
+          <a:off x="27789840" y="5489640"/>
+          <a:ext cx="3265560" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3503,26 +3468,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>721800</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>80640</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>800640</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>79560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>784800</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>761400</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>79920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="46" name="CustomShape 1"/>
+        <xdr:cNvPr id="40" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="27797400" y="5490360"/>
-          <a:ext cx="3267360" cy="360"/>
+        <a:xfrm>
+          <a:off x="29469960" y="17710920"/>
+          <a:ext cx="30388680" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3567,26 +3532,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>800640</xdr:colOff>
-      <xdr:row>94</xdr:row>
-      <xdr:rowOff>79560</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>665280</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>88920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>761760</xdr:colOff>
-      <xdr:row>94</xdr:row>
-      <xdr:rowOff>79920</xdr:rowOff>
+      <xdr:colOff>684720</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>89280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="47" name="CustomShape 1"/>
+        <xdr:cNvPr id="41" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="29478240" y="17710920"/>
-          <a:ext cx="30401280" cy="360"/>
+        <a:xfrm flipH="1">
+          <a:off x="26131680" y="18329760"/>
+          <a:ext cx="33650280" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3632,25 +3597,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>666000</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>88920</xdr:rowOff>
+      <xdr:colOff>743040</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>89280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>89280</xdr:rowOff>
+      <xdr:colOff>751680</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>89640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="48" name="CustomShape 1"/>
+        <xdr:cNvPr id="42" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="26139600" y="18329760"/>
-          <a:ext cx="33663960" cy="360"/>
+        <a:xfrm>
+          <a:off x="26209440" y="18482400"/>
+          <a:ext cx="33639480" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3695,26 +3660,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>743040</xdr:colOff>
-      <xdr:row>98</xdr:row>
-      <xdr:rowOff>89280</xdr:rowOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>678240</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>86040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>752040</xdr:colOff>
-      <xdr:row>98</xdr:row>
-      <xdr:rowOff>89640</xdr:rowOff>
+      <xdr:colOff>716040</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>86400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="49" name="CustomShape 1"/>
+        <xdr:cNvPr id="43" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="26216640" y="18482400"/>
-          <a:ext cx="33653160" cy="360"/>
+        <a:xfrm flipV="1">
+          <a:off x="58174200" y="19088640"/>
+          <a:ext cx="1639080" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3759,26 +3724,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>678240</xdr:colOff>
-      <xdr:row>100</xdr:row>
-      <xdr:rowOff>86760</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>714600</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>88920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>716400</xdr:colOff>
-      <xdr:row>100</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>686520</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>89280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="50" name="CustomShape 1"/>
+        <xdr:cNvPr id="44" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="58194000" y="19089360"/>
-          <a:ext cx="1640160" cy="360"/>
+        <a:xfrm flipH="1">
+          <a:off x="10244520" y="19701360"/>
+          <a:ext cx="51140880" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3823,26 +3788,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>714600</xdr:colOff>
-      <xdr:row>102</xdr:row>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>676800</xdr:colOff>
+      <xdr:row>104</xdr:row>
       <xdr:rowOff>88920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>686880</xdr:colOff>
-      <xdr:row>102</xdr:row>
+      <xdr:colOff>714600</xdr:colOff>
+      <xdr:row>104</xdr:row>
       <xdr:rowOff>89280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="51" name="CustomShape 1"/>
+        <xdr:cNvPr id="45" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="10247040" y="19701360"/>
-          <a:ext cx="51159600" cy="360"/>
+          <a:off x="59774040" y="20006280"/>
+          <a:ext cx="1639440" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3887,26 +3852,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>-40862520</xdr:colOff>
-      <xdr:row>103</xdr:row>
-      <xdr:rowOff>73440</xdr:rowOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>743400</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>88920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>777240</xdr:colOff>
-      <xdr:row>103</xdr:row>
-      <xdr:rowOff>73800</xdr:rowOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>780840</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>89280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="52" name="CustomShape 1"/>
+        <xdr:cNvPr id="46" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="-40862520" y="19837800"/>
-          <a:ext cx="51172200" cy="360"/>
+        <a:xfrm flipH="1">
+          <a:off x="58239360" y="20158560"/>
+          <a:ext cx="1638720" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3951,26 +3916,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>676800</xdr:colOff>
-      <xdr:row>104</xdr:row>
-      <xdr:rowOff>88920</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>541800</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>63720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>714960</xdr:colOff>
-      <xdr:row>104</xdr:row>
-      <xdr:rowOff>89280</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>675360</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>75600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="53" name="CustomShape 1"/>
+        <xdr:cNvPr id="47" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="59794560" y="20006280"/>
-          <a:ext cx="1640160" cy="360"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="51631920" y="20285640"/>
+          <a:ext cx="3336480" cy="11880"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4015,26 +3980,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>743400</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>88920</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>681120</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>86040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>781200</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>89280</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>744840</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>86400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="54" name="CustomShape 1"/>
+        <xdr:cNvPr id="48" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="58259160" y="20158560"/>
-          <a:ext cx="1639800" cy="360"/>
+        <a:xfrm flipV="1">
+          <a:off x="46966680" y="20917440"/>
+          <a:ext cx="8071200" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4079,26 +4044,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>541800</xdr:colOff>
-      <xdr:row>106</xdr:row>
-      <xdr:rowOff>64440</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>685440</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>88920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>675720</xdr:colOff>
-      <xdr:row>106</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>733680</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>89280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="55" name="CustomShape 1"/>
+        <xdr:cNvPr id="49" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="51648840" y="20286360"/>
-          <a:ext cx="3338280" cy="12240"/>
+        <a:xfrm flipH="1">
+          <a:off x="54978480" y="21530160"/>
+          <a:ext cx="8055360" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4143,26 +4108,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>681120</xdr:colOff>
-      <xdr:row>109</xdr:row>
-      <xdr:rowOff>86760</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>724320</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>89280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
-      <xdr:colOff>745200</xdr:colOff>
-      <xdr:row>109</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
+      <xdr:colOff>761400</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>89640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="56" name="CustomShape 1"/>
+        <xdr:cNvPr id="50" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="46981800" y="20918160"/>
-          <a:ext cx="8074800" cy="360"/>
+        <a:xfrm flipH="1">
+          <a:off x="50212800" y="21682800"/>
+          <a:ext cx="4841640" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4207,26 +4172,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>685440</xdr:colOff>
-      <xdr:row>111</xdr:row>
-      <xdr:rowOff>88920</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>764640</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>86400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>734040</xdr:colOff>
-      <xdr:row>111</xdr:row>
-      <xdr:rowOff>89280</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>802080</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>86760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="57" name="CustomShape 1"/>
+        <xdr:cNvPr id="51" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="54996840" y="21530160"/>
-          <a:ext cx="8058960" cy="360"/>
+        <a:xfrm flipV="1">
+          <a:off x="48651840" y="23051160"/>
+          <a:ext cx="1638720" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4272,25 +4237,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>725040</xdr:colOff>
-      <xdr:row>112</xdr:row>
-      <xdr:rowOff>89280</xdr:rowOff>
+      <xdr:colOff>707760</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>86400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>762480</xdr:colOff>
-      <xdr:row>112</xdr:row>
-      <xdr:rowOff>89640</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>745200</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>86760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="58" name="CustomShape 1"/>
+        <xdr:cNvPr id="52" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="50230080" y="21682800"/>
-          <a:ext cx="4843800" cy="360"/>
+        <a:xfrm flipV="1">
+          <a:off x="50196240" y="23508360"/>
+          <a:ext cx="1639080" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4335,26 +4300,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>764640</xdr:colOff>
-      <xdr:row>118</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>714240</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>79560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>802440</xdr:colOff>
-      <xdr:row>118</xdr:row>
-      <xdr:rowOff>87480</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>704520</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>79920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="59" name="CustomShape 1"/>
+        <xdr:cNvPr id="53" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="48667680" y="23051880"/>
-          <a:ext cx="1639800" cy="360"/>
+        <a:xfrm flipH="1">
+          <a:off x="12965040" y="23806800"/>
+          <a:ext cx="40430880" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4397,134 +4362,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>707760</xdr:colOff>
-      <xdr:row>120</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>745560</xdr:colOff>
-      <xdr:row>120</xdr:row>
-      <xdr:rowOff>87480</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="60" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="50212800" y="23509080"/>
-          <a:ext cx="1639800" cy="360"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="21600" h="21600">
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="21600" y="21600"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="34920">
-          <a:solidFill>
-            <a:srgbClr val="4a7ebb"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd len="med" type="oval" w="med"/>
-          <a:tailEnd len="med" type="triangle" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>714240</xdr:colOff>
-      <xdr:row>122</xdr:row>
-      <xdr:rowOff>79560</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>704880</xdr:colOff>
-      <xdr:row>122</xdr:row>
-      <xdr:rowOff>79920</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="61" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="12967560" y="23806800"/>
-          <a:ext cx="40446720" cy="360"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="21600" h="21600">
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="21600" y="21600"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="34920">
-          <a:solidFill>
-            <a:srgbClr val="4a7ebb"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd len="med" type="oval" w="med"/>
-          <a:tailEnd len="med" type="triangle" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4535,8 +4372,8 @@
   </sheetPr>
   <dimension ref="A2:AO123"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="5" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="5" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="C87" activeCellId="0" sqref="C87"/>
     </sheetView>
@@ -4547,7 +4384,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="1" width="22.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="9" style="1" width="22.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="1" width="22.7"/>
@@ -5798,23 +5635,548 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="55.7"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="19"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="22"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" s="25"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="22"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="25"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="D29" s="35" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" s="37" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="C31" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="D31" s="37"/>
+    </row>
+    <row r="32" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="C32" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="D32" s="41" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="C33" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="D33" s="41"/>
+    </row>
+    <row r="34" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="D34" s="30" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="D35" s="41" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="C36" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="D36" s="41"/>
+    </row>
+    <row r="37" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="C37" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" s="37" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="B38" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="C38" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="D38" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D37:D38"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -5843,4 +6205,30 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.54"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Order level strate identifier application.
</commit_message>
<xml_diff>
--- a/RMSXRouteFillTest/RMSXRouteFillTest_SequenceDiagram.xlsx
+++ b/RMSXRouteFillTest/RMSXRouteFillTest_SequenceDiagram.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="183">
   <si>
     <t>RouteFillTest</t>
   </si>
@@ -572,13 +572,16 @@
   </si>
   <si>
     <t>Broker rejected the order from sent status</t>
+  </si>
+  <si>
+    <t>Route State Transitions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -605,6 +608,13 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -817,41 +827,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -936,6 +913,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4838,615 +4849,608 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" style="12" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="12" customWidth="1"/>
-    <col min="4" max="7" width="22.7109375" style="12" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="12" customWidth="1"/>
-    <col min="9" max="14" width="22.7109375" style="12" customWidth="1"/>
-    <col min="15" max="15" width="28.42578125" style="12" customWidth="1"/>
-    <col min="16" max="1025" width="22.7109375" style="12" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" style="1" customWidth="1"/>
+    <col min="4" max="7" width="22.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="1" customWidth="1"/>
+    <col min="9" max="14" width="22.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="28.42578125" style="1" customWidth="1"/>
+    <col min="16" max="1025" width="22.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="10" t="s">
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10" t="s">
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="10"/>
-      <c r="AC2" s="10"/>
-      <c r="AD2" s="10"/>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10"/>
-      <c r="AG2" s="10"/>
-      <c r="AH2" s="10"/>
-      <c r="AI2" s="10"/>
-      <c r="AJ2" s="10"/>
-      <c r="AK2" s="10"/>
-      <c r="AL2" s="10"/>
-      <c r="AM2" s="10"/>
-      <c r="AN2" s="10"/>
-      <c r="AO2" s="14"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+      <c r="X2" s="40"/>
+      <c r="Y2" s="40"/>
+      <c r="Z2" s="40"/>
+      <c r="AA2" s="40"/>
+      <c r="AB2" s="40"/>
+      <c r="AC2" s="40"/>
+      <c r="AD2" s="40"/>
+      <c r="AE2" s="40"/>
+      <c r="AF2" s="40"/>
+      <c r="AG2" s="40"/>
+      <c r="AH2" s="40"/>
+      <c r="AI2" s="40"/>
+      <c r="AJ2" s="40"/>
+      <c r="AK2" s="40"/>
+      <c r="AL2" s="40"/>
+      <c r="AM2" s="40"/>
+      <c r="AN2" s="40"/>
+      <c r="AO2" s="3"/>
     </row>
     <row r="3" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10" t="s">
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10" t="s">
+      <c r="I3" s="40"/>
+      <c r="J3" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10" t="s">
+      <c r="K3" s="40"/>
+      <c r="L3" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10" t="s">
+      <c r="N3" s="40"/>
+      <c r="O3" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="P3" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10" t="s">
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="S3" s="10"/>
-      <c r="T3" s="8" t="s">
+      <c r="S3" s="40"/>
+      <c r="T3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="10" t="s">
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="8" t="s">
+      <c r="X3" s="40"/>
+      <c r="Y3" s="40"/>
+      <c r="Z3" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="AA3" s="10" t="s">
+      <c r="AA3" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="AB3" s="10"/>
-      <c r="AC3" s="10" t="s">
+      <c r="AB3" s="40"/>
+      <c r="AC3" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="AD3" s="11" t="s">
+      <c r="AD3" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="AE3" s="11"/>
-      <c r="AF3" s="11"/>
-      <c r="AG3" s="11"/>
-      <c r="AH3" s="11"/>
-      <c r="AI3" s="11"/>
-      <c r="AJ3" s="11"/>
-      <c r="AK3" s="10" t="s">
+      <c r="AE3" s="41"/>
+      <c r="AF3" s="41"/>
+      <c r="AG3" s="41"/>
+      <c r="AH3" s="41"/>
+      <c r="AI3" s="41"/>
+      <c r="AJ3" s="41"/>
+      <c r="AK3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="AL3" s="10"/>
-      <c r="AM3" s="10"/>
-      <c r="AN3" s="10"/>
-      <c r="AO3" s="14"/>
+      <c r="AL3" s="40"/>
+      <c r="AM3" s="40"/>
+      <c r="AN3" s="40"/>
+      <c r="AO3" s="3"/>
     </row>
     <row r="4" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="10"/>
-      <c r="AB4" s="10"/>
-      <c r="AC4" s="10"/>
-      <c r="AD4" s="7"/>
-      <c r="AE4" s="7"/>
-      <c r="AF4" s="10" t="s">
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="39"/>
+      <c r="V4" s="39"/>
+      <c r="W4" s="40"/>
+      <c r="X4" s="40"/>
+      <c r="Y4" s="40"/>
+      <c r="Z4" s="39"/>
+      <c r="AA4" s="40"/>
+      <c r="AB4" s="40"/>
+      <c r="AC4" s="40"/>
+      <c r="AD4" s="42"/>
+      <c r="AE4" s="42"/>
+      <c r="AF4" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="AG4" s="10"/>
-      <c r="AH4" s="10"/>
-      <c r="AI4" s="10"/>
-      <c r="AJ4" s="10"/>
-      <c r="AK4" s="10"/>
-      <c r="AL4" s="10"/>
-      <c r="AM4" s="10"/>
-      <c r="AN4" s="10"/>
-      <c r="AO4" s="14"/>
+      <c r="AG4" s="40"/>
+      <c r="AH4" s="40"/>
+      <c r="AI4" s="40"/>
+      <c r="AJ4" s="40"/>
+      <c r="AK4" s="40"/>
+      <c r="AL4" s="40"/>
+      <c r="AM4" s="40"/>
+      <c r="AN4" s="40"/>
+      <c r="AO4" s="3"/>
     </row>
     <row r="5" spans="1:41" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="15" t="s">
+      <c r="A5" s="43"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="10"/>
-      <c r="M5" s="13" t="s">
+      <c r="L5" s="40"/>
+      <c r="M5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N5" s="13" t="s">
+      <c r="N5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="13" t="s">
+      <c r="O5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="P5" s="13" t="s">
+      <c r="P5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Q5" s="13" t="s">
+      <c r="Q5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="R5" s="13" t="s">
+      <c r="R5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S5" s="13" t="s">
+      <c r="S5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="T5" s="13" t="s">
+      <c r="T5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="U5" s="13" t="s">
+      <c r="U5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="V5" s="13" t="s">
+      <c r="V5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="W5" s="13" t="s">
+      <c r="W5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="X5" s="13" t="s">
+      <c r="X5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="Y5" s="13" t="s">
+      <c r="Y5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="13" t="s">
+      <c r="Z5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AA5" s="13" t="s">
+      <c r="AA5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AB5" s="13" t="s">
+      <c r="AB5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AC5" s="13" t="s">
+      <c r="AC5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AD5" s="13" t="s">
+      <c r="AD5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AE5" s="13" t="s">
+      <c r="AE5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AF5" s="13" t="s">
+      <c r="AF5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AG5" s="13" t="s">
+      <c r="AG5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AH5" s="13" t="s">
+      <c r="AH5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AI5" s="13" t="s">
+      <c r="AI5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AJ5" s="13" t="s">
+      <c r="AJ5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AK5" s="13" t="s">
+      <c r="AK5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AL5" s="13" t="s">
+      <c r="AL5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AM5" s="13" t="s">
+      <c r="AM5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AN5" s="13" t="s">
+      <c r="AN5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AO5" s="14"/>
+      <c r="AO5" s="3"/>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:41" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="H12" s="17" t="s">
+      <c r="H12" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="H14" s="17"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="H15" s="17"/>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:41" ht="24" x14ac:dyDescent="0.25">
-      <c r="H16" s="17" t="s">
+      <c r="H16" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
+    <row r="22" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
+    <row r="23" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
+    <row r="24" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+    <row r="31" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="A37" s="17" t="s">
+    <row r="33" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
+    <row r="38" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
+    <row r="40" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="A45" s="17" t="s">
+    <row r="41" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:1" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:1" s="17" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="A47" s="17" t="s">
+    <row r="46" spans="1:1" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:1" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:1" s="17" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="A48" s="17" t="s">
+    <row r="48" spans="1:1" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="2:12" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="2:12" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="B50" s="17" t="s">
+    <row r="49" spans="2:12" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="2:12" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="B50" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="L50" s="17" t="s">
+      <c r="L50" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="2:12" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="2:12" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="2:12" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="C53" s="17" t="s">
+    <row r="51" spans="2:12" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="2:12" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="2:12" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="C53" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="54" spans="2:12" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="C54" s="17" t="s">
+    <row r="54" spans="2:12" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="C54" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="2:12" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="2:12" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="2:12" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="2:12" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="2:12" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="2:12" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="C60" s="17" t="s">
+    <row r="55" spans="2:12" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="2:12" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="2:12" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="2:12" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="2:12" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="2:12" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="C60" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="2:12" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="2:12" s="17" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="D62" s="17" t="s">
+    <row r="61" spans="2:12" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="2:12" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="D62" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="63" spans="2:12" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="2:12" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="3:30" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="3:30" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="3:30" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="3:30" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="3:30" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="3:30" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="C70" s="17" t="s">
+    <row r="63" spans="2:12" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="2:12" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="3:30" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="3:30" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="3:30" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="3:30" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="3:30" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="3:30" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="C70" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="3:30" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="3:30" s="17" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C72" s="17" t="s">
+    <row r="71" spans="3:30" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="3:30" s="6" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C72" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="3:30" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="3:30" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="Y74" s="17" t="s">
+    <row r="73" spans="3:30" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="3:30" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="Y74" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="3:30" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="3:30" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="3:30" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="3:30" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="3:30" s="17" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="AD79" s="17" t="s">
+    <row r="75" spans="3:30" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="3:30" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="3:30" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="3:30" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="3:30" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="AD79" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="80" spans="3:30" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="81" spans="3:38" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="Y81" s="18" t="s">
+    <row r="80" spans="3:30" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="3:38" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="Y81" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="82" spans="3:38" s="17" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="Y82" s="17" t="s">
+    <row r="82" spans="3:38" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="Y82" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="83" spans="3:38" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="3:38" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="3:38" s="17" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="Y85" s="17" t="s">
+    <row r="83" spans="3:38" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="3:38" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="3:38" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="Y85" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="86" spans="3:38" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="3:38" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="C87" s="17" t="s">
+    <row r="86" spans="3:38" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="3:38" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="C87" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="88" spans="3:38" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="AF88" s="17" t="s">
+    <row r="88" spans="3:38" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="AF88" s="6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="89" spans="3:38" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="90" spans="3:38" s="17" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="AI90" s="17" t="s">
+    <row r="89" spans="3:38" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="3:38" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="AI90" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="91" spans="3:38" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="92" spans="3:38" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="93" spans="3:38" s="17" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="AL93" s="17" t="s">
+    <row r="91" spans="3:38" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="3:38" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="3:38" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="AL93" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="94" spans="3:38" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="95" spans="3:38" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="3:38" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="AL96" s="17" t="s">
+    <row r="94" spans="3:38" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="3:38" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="3:38" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="AL96" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="97" spans="35:40" s="17" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="AL97" s="17" t="s">
+    <row r="97" spans="35:40" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="AL97" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="98" spans="35:40" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="99" spans="35:40" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="100" spans="35:40" s="17" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="AL100" s="17" t="s">
+    <row r="98" spans="35:40" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="99" spans="35:40" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="35:40" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="AL100" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="101" spans="35:40" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="102" spans="35:40" s="17" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="AM102" s="17" t="s">
+    <row r="101" spans="35:40" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="35:40" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="AM102" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="103" spans="35:40" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="104" spans="35:40" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="105" spans="35:40" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="35:40" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="35:40" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="108" spans="35:40" s="17" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="AI108" s="17" t="s">
+    <row r="103" spans="35:40" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="104" spans="35:40" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="35:40" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="35:40" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="35:40" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="35:40" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="AI108" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="109" spans="35:40" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="AI109" s="17" t="s">
+    <row r="109" spans="35:40" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="AI109" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="110" spans="35:40" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="35:40" s="17" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="AN111" s="17" t="s">
+    <row r="110" spans="35:40" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="35:40" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="AN111" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="112" spans="35:40" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="113" spans="32:34" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="114" spans="32:34" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="115" spans="32:34" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="AF115" s="17" t="s">
+    <row r="112" spans="35:40" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="113" spans="32:34" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="114" spans="32:34" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="32:34" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="AF115" s="6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="116" spans="32:34" s="17" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="AF116" s="17" t="s">
+    <row r="116" spans="32:34" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="AF116" s="6" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="117" spans="32:34" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="32:34" s="17" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="AF118" s="17" t="s">
+    <row r="117" spans="32:34" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="32:34" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="AF118" s="6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="119" spans="32:34" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="32:34" s="17" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="AG120" s="17" t="s">
+    <row r="119" spans="32:34" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="32:34" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="AG120" s="6" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="121" spans="32:34" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="32:34" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="AH122" s="17" t="s">
+    <row r="121" spans="32:34" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="32:34" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="AH122" s="6" t="s">
         <v>90</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AB4"/>
-    <mergeCell ref="AC3:AC4"/>
-    <mergeCell ref="AD3:AJ3"/>
-    <mergeCell ref="AK3:AN4"/>
-    <mergeCell ref="AD4:AE4"/>
-    <mergeCell ref="AF4:AJ4"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="O2:AN2"/>
@@ -5463,6 +5467,13 @@
     <mergeCell ref="R3:S4"/>
     <mergeCell ref="T3:V4"/>
     <mergeCell ref="W3:Y4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AB4"/>
+    <mergeCell ref="AC3:AC4"/>
+    <mergeCell ref="AD3:AJ3"/>
+    <mergeCell ref="AK3:AN4"/>
+    <mergeCell ref="AD4:AE4"/>
+    <mergeCell ref="AF4:AJ4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5472,11 +5483,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5488,738 +5497,743 @@
     <col min="6" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="50" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B3" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C3" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D3" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E3" s="49" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="48"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B5" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C5" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D5" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E5" s="10" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B6" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C6" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D6" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E6" s="14" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B7" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C7" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D7" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E7" s="10" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B8" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C8" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D8" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E8" s="46" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B9" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C9" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B10" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C10" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D10" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E10" s="47" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B11" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C11" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B12" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C12" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D12" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E12" s="46" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B13" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C13" s="16">
         <v>0</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B14" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C14" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D14" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E14" s="47" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="C13" s="31">
-        <v>0</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="C14" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="E14" s="34" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="20">
+        <v>0</v>
+      </c>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B16" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C16" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D17" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="E15" s="36" t="s">
+      <c r="E17" s="25" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B18" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C18" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D18" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="E18" s="23" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B19" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C19" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D19" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E19" s="10" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B20" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C20" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D20" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="E18" s="34" t="s">
+      <c r="E20" s="23" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B21" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C21" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D21" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E21" s="10" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B22" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="C22" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D22" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="E20" s="34" t="s">
+      <c r="E22" s="23" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B23" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C23" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="D23" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="E21" s="21" t="s">
+      <c r="E23" s="10" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="B22" s="33" t="s">
+      <c r="B24" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C24" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D24" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="E22" s="34" t="s">
+      <c r="E24" s="23" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B25" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C25" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="D25" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="E23" s="21" t="s">
+      <c r="E25" s="10" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="33" t="s">
+      <c r="B26" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="C24" s="33" t="s">
+      <c r="C26" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="D26" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="E24" s="34" t="s">
+      <c r="E26" s="23" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B27" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C27" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="D27" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="E27" s="10" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="32" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="B26" s="33" t="s">
+      <c r="B28" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="C26" s="33" t="s">
+      <c r="C28" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="D26" s="34" t="s">
+      <c r="D28" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="E26" s="34" t="s">
+      <c r="E28" s="23" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B29" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C29" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D29" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E29" s="10" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="37" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" s="38" t="s">
-        <v>145</v>
-      </c>
-      <c r="C28" s="38" t="s">
-        <v>148</v>
-      </c>
-      <c r="D28" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="E28" s="39" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="B29" s="40" t="s">
-        <v>148</v>
-      </c>
-      <c r="C29" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="D30" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="E31" s="45" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="B30" s="41" t="s">
+      <c r="B32" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="C30" s="41" t="s">
+      <c r="C32" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="42" t="s">
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="B31" s="43" t="s">
+      <c r="B33" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="C31" s="43" t="s">
+      <c r="C33" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D33" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E33" s="44" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="44" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="B32" s="45" t="s">
+      <c r="B34" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="C32" s="45" t="s">
+      <c r="C34" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="32" t="s">
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="B33" s="33" t="s">
+      <c r="B35" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="C33" s="33" t="s">
+      <c r="C35" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="D33" s="34" t="s">
+      <c r="D35" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="E33" s="34" t="s">
+      <c r="E35" s="23" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="42" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="B34" s="43" t="s">
+      <c r="B36" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="C34" s="43" t="s">
+      <c r="C36" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D36" s="44" t="s">
         <v>161</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E36" s="44" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="44" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="B35" s="45" t="s">
+      <c r="B37" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="C35" s="45" t="s">
+      <c r="C37" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="22" t="s">
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B36" s="40" t="s">
+      <c r="B38" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="C36" s="40" t="s">
+      <c r="C38" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D38" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E38" s="45" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="26" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="B37" s="41" t="s">
+      <c r="B39" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="C37" s="41" t="s">
+      <c r="C39" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
+      <c r="D39" s="45"/>
+      <c r="E39" s="45"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B40" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="C40" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="D38" s="21" t="s">
+      <c r="D40" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="E38" s="21" t="s">
+      <c r="E40" s="10" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="32" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="B39" s="33" t="s">
+      <c r="B41" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="C39" s="33" t="s">
+      <c r="C41" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="D39" s="34" t="s">
+      <c r="D41" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="E39" s="34" t="s">
+      <c r="E41" s="23" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B40" s="20" t="s">
+      <c r="B42" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="20" t="s">
+      <c r="C42" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D40" s="21" t="s">
+      <c r="D42" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="E40" s="21" t="s">
+      <c r="E42" s="10" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="46" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="B41" s="47" t="s">
+      <c r="B43" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="C41" s="47" t="s">
+      <c r="C43" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="D41" s="34" t="s">
+      <c r="D43" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="E41" s="34" t="s">
+      <c r="E43" s="23" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="48" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="B42" s="49" t="s">
+      <c r="B44" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C42" s="49" t="s">
+      <c r="C44" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D44" t="s">
         <v>172</v>
       </c>
-      <c r="E42" s="21" t="s">
+      <c r="E44" s="10" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="46" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="B43" s="47" t="s">
+      <c r="B45" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="C43" s="33" t="s">
+      <c r="C45" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="D43" s="46" t="s">
+      <c r="D45" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="E43" s="46" t="s">
+      <c r="E45" s="35" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="48" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="B44" s="49" t="s">
+      <c r="B46" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="C44" s="49" t="s">
+      <c r="C46" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="D44" s="48" t="s">
+      <c r="D46" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="E44" s="48" t="s">
+      <c r="E46" s="37" t="s">
         <v>177</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="D31:D32"/>
     <mergeCell ref="E31:E32"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
     <mergeCell ref="D36:D37"/>
     <mergeCell ref="E36:E37"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>